<commit_message>
validaattori testit etc Github sekos
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6466E4-0EEE-45DE-BF84-5D3BC3FC29B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5D7BF8-6EB8-42ED-92C7-676E247E96E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="2310" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Päivä</t>
   </si>
@@ -53,22 +53,31 @@
     <t>Firebasen opettelua ja pystyyn pistämistä</t>
   </si>
   <si>
-    <t>Firebasen opettelua ja mapsAPIn toiminnan selvittämistä</t>
-  </si>
-  <si>
-    <t>Three.js:n harjoittelua ja demoamista. Mahdollisesti kiipeily seinän tekemiseen applikaatioon.</t>
-  </si>
-  <si>
     <t>Three.js harjottelua</t>
   </si>
   <si>
-    <t>Blender objectien ja three.js:n yhteen sovittelua</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stacki muutettu firebasen maksullisten cloud funktio muutosten takia. Uus stacki front: react, redux, javascript/three.js back: node </t>
   </si>
   <si>
     <t>Stacki vaihettu taas: hostaus: firebase ja login: Oauth</t>
+  </si>
+  <si>
+    <t>Firebase with react</t>
+  </si>
+  <si>
+    <t>3d mallien importtaaminen ja menun rakentaminen</t>
+  </si>
+  <si>
+    <t>Three.js:n harjoittelua ja demoamista. Mahdollisesti animaatioiden tekoa sivulle</t>
+  </si>
+  <si>
+    <t>Firebasen opettelua</t>
+  </si>
+  <si>
+    <t>Three.js:n objectien muodostamista</t>
+  </si>
+  <si>
+    <t>Databasen rakentamista, validaattoreidenn tekemistä</t>
   </si>
 </sst>
 </file>
@@ -77,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,8 +129,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -130,10 +139,10 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -161,10 +170,10 @@
   <autoFilter ref="A1:C42" xr:uid="{B30BF170-5FD0-4BDF-BBEC-E02979536BF7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2B7E2D50-4609-4344-9894-701204051296}" name="Päivä" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F3C4214F-98CB-4F08-9353-9A647E484DFD}" name="Aika (h)" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{F3C4214F-98CB-4F08-9353-9A647E484DFD}" name="Aika (h)" dataDxfId="1">
       <calculatedColumnFormula>SUM(B$2:B$41)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1F33100E-4C74-4639-8B4B-8B49CE3360E9}" name="Mitä tein" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1F33100E-4C74-4639-8B4B-8B49CE3360E9}" name="Mitä tein" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -470,7 +479,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44021</v>
       </c>
@@ -510,10 +519,10 @@
         <v>1.5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44021</v>
       </c>
@@ -521,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,7 +541,7 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,10 +549,10 @@
         <v>44022</v>
       </c>
       <c r="B6" s="6">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -554,7 +563,7 @@
         <v>1.25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -565,23 +574,41 @@
         <v>0.25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
+      <c r="A9" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B10" s="6">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44033</v>
+      </c>
+      <c r="B11" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -739,7 +766,7 @@
       </c>
       <c r="B42" s="6">
         <f t="shared" ref="B42" si="0">SUM(B$2:B$41)</f>
-        <v>14.5</v>
+        <v>22.5</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Oauthin toiminnan selvittämistä ja usereiden tallentamisen ja toiminnan suunnittelua
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF0617-ABFE-4C03-9055-4F8A31683ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B939D820-9F94-47CA-8371-E68E6280D770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="-28410" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Päivä</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>CommentSection alustettu kommentoiminen mahdollista ja oauth käyttöön</t>
+  </si>
+  <si>
+    <t>Oauthin toiminnan selvittämistä ja usereiden tallentamisen ja toiminnan suunnittelua</t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,10 +840,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -933,7 +942,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>46.25</v>
+        <v>49.25</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Usereiden luonti ja käyttäjänhallinan selvittely
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445AB175-EB77-4FA2-A1FE-5D134C917748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6D09E2-5F5A-4C34-971B-03C341303B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28410" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Päivä</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>User mallien toimintaa ja discriminaattoreiden tekoa eri käyttäjille</t>
+  </si>
+  <si>
+    <t>User malleja toimintaan - thirdparty login ja järkevän tavan etsintää, toteuttamaan käyttäjänhallintaa</t>
   </si>
 </sst>
 </file>
@@ -621,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K30" sqref="K29:K30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +877,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B23" s="6">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -960,7 +969,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>50.75</v>
+        <v>56.75</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Google Loginnin ja oauthin toimintaan saamista
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B61B6BA-1981-4B78-93EA-BC78DF07E701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71196B84-CDFE-40CA-98B9-ABA9516FACCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28410" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Päivä</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>GoogleLoginnin kehittämistä ja validoimiseen tutustumista</t>
+  </si>
+  <si>
+    <t>GoogleLoginnin/Oauthin toimintaan saamista</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,9 +906,15 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B25" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -978,7 +987,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>59.25</v>
+        <v>62.75</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Käyttäjänhallinnan mahdollistamista, kuvien hallinnan mahdollistamista
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B053019-AA7C-4C8E-8284-E8D3BD25290D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502D0BD-C47D-44EF-A63F-819A524E3684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28410" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Päivä</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Google login, varmennus, on-site login ja tokenit toimimaan</t>
+  </si>
+  <si>
+    <t>Käyttäjänhallinnan mahdollistamista, kuvien hallinnan mahdollistamista</t>
   </si>
 </sst>
 </file>
@@ -634,7 +637,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,10 +933,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="4"/>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -996,7 +1005,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>68.75</v>
+        <v>72.25</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Logon suunnittelu, kuvan lataamisen ja optimointi
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745ACC4D-53B0-4B57-9AE5-BA7AA339447B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1516F647-8979-4E6D-B6A5-82D76319BC82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Päivä</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Logo suunnittelua</t>
+  </si>
+  <si>
+    <t>Logon suunnittelu, kuvan lataamisen ja optimointi</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,10 +998,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="4"/>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B31" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1041,7 +1050,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>79.25</v>
+        <v>81.75</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Kuvien lataaminen serveriltä sekä productio version testaus
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F5F392-E957-4BD0-BE94-587EF0FEC54C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F34A43-00B1-4B3F-A2AC-1802437D2C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2610" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Päivä</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">Serveri puolen kuvien kompressoimisen tekeminen ja userit näkymään </t>
+  </si>
+  <si>
+    <t>Kuvien lataaminen serveriltä sekä productio version testaus</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,10 +1026,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="4"/>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B33" s="6">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1059,7 +1068,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>83.75</v>
+        <v>87.75</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
usernamen generoimista ja cookieiden käyttöä localstoragen sijasta.
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F34A43-00B1-4B3F-A2AC-1802437D2C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5224F97C-A96E-43D6-8D1C-CC96C76DE155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Päivä</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Kuvien lataaminen serveriltä sekä productio version testaus</t>
+  </si>
+  <si>
+    <t>usernamen generoimista ja cookieiden käyttöä localstoragen sijasta.</t>
   </si>
 </sst>
 </file>
@@ -663,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,10 +1040,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="4"/>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B34" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -1068,7 +1077,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>87.75</v>
+        <v>90.25</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Backendin testaamista ja confirmaatio sähköpostin lähettämistä
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5224F97C-A96E-43D6-8D1C-CC96C76DE155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2338C9EA-574C-49B3-BA43-AF2A23F62704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Päivä</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>usernamen generoimista ja cookieiden käyttöä localstoragen sijasta.</t>
+  </si>
+  <si>
+    <t>Backendin testaamista ja confirmaatio sähköpostin lähettämistä</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,10 +1054,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="4"/>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B35" s="6">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -1077,7 +1086,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>90.25</v>
+        <v>93.25</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
User update toimimaan ja tokenien muuttelua
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC729025-6716-466F-9611-9684A10C76BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED5FC0-D91C-4A28-AF99-7A291C8D6355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Päivä</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Backarin testaamista postmanilla</t>
+  </si>
+  <si>
+    <t>User update toimimaan ja tokenien muuttelua</t>
   </si>
 </sst>
 </file>
@@ -673,7 +676,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,9 +1083,15 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B37" s="6">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -1095,7 +1104,7 @@
       </c>
       <c r="B39" s="6">
         <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>96.25</v>
+        <v>98.25</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Frontin layout suunnittelua  ja update työaika
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED5FC0-D91C-4A28-AF99-7A291C8D6355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4625BF-955B-4B35-B1B4-AA87B986FE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Päivä</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Aika (h)</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Done!</t>
-  </si>
-  <si>
     <t>Firebasen opettelua ja pystyyn pistämistä</t>
   </si>
   <si>
@@ -156,6 +150,9 @@
   </si>
   <si>
     <t>User update toimimaan ja tokenien muuttelua</t>
+  </si>
+  <si>
+    <t>Change password ja reset password toimintaan sekä frontin layout suunnittelua.</t>
   </si>
 </sst>
 </file>
@@ -363,8 +360,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E38EF31-D64B-4356-982E-F2FAEB215E8B}" name="Table1" displayName="Table1" ref="A1:C39" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C39" xr:uid="{B30BF170-5FD0-4BDF-BBEC-E02979536BF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E38EF31-D64B-4356-982E-F2FAEB215E8B}" name="Table1" displayName="Table1" ref="A1:C60" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C60" xr:uid="{B30BF170-5FD0-4BDF-BBEC-E02979536BF7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2B7E2D50-4609-4344-9894-701204051296}" name="Päivä" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{F3C4214F-98CB-4F08-9353-9A647E484DFD}" name="Aika (h)" dataDxfId="1">
@@ -673,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +702,7 @@
         <v>1.5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,7 +713,7 @@
         <v>1.5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -738,7 +735,7 @@
         <v>1.25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -749,7 +746,7 @@
         <v>0.25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +757,7 @@
         <v>1.5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -771,7 +768,7 @@
         <v>4.5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -782,7 +779,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,7 +790,7 @@
         <v>1.5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -804,7 +801,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -826,7 +823,7 @@
         <v>1.5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,7 +834,7 @@
         <v>1.25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,7 +856,7 @@
         <v>1.5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,7 +878,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -892,7 +889,7 @@
         <v>2.5</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -903,7 +900,7 @@
         <v>3.5</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -914,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="33" x14ac:dyDescent="0.25">
@@ -925,7 +922,7 @@
         <v>1.5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -936,7 +933,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -947,7 +944,7 @@
         <v>2.5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +955,7 @@
         <v>3.5</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -969,7 +966,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -980,7 +977,7 @@
         <v>3.5</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -991,7 +988,7 @@
         <v>2.5</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1002,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,7 +1010,7 @@
         <v>1.5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1024,7 +1021,7 @@
         <v>2.5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1035,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1046,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1057,7 +1054,7 @@
         <v>2.5</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1068,7 +1065,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,7 +1076,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,25 +1087,132 @@
         <v>2</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="4"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B38" s="6">
+        <v>6</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="6">
-        <f t="shared" ref="B39" si="0">SUM(B$2:B$38)</f>
-        <v>98.25</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="6">
+        <f>SUM(B$2:B$59)</f>
+        <v>104.25</v>
+      </c>
+      <c r="C60" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adobe xd ja wireframee
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4625BF-955B-4B35-B1B4-AA87B986FE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8015B0ED-F755-41E1-B53E-551A5556C0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Päivä</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Change password ja reset password toimintaan sekä frontin layout suunnittelua.</t>
+  </si>
+  <si>
+    <t>Sivun wireframea ja adobe xd:hen tutustumista</t>
   </si>
 </sst>
 </file>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,9 +1105,15 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B39" s="6">
+        <v>5</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
@@ -1210,7 +1219,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="6">
         <f>SUM(B$2:B$59)</f>
-        <v>104.25</v>
+        <v>109.25</v>
       </c>
       <c r="C60" s="3"/>
     </row>

</xml_diff>

<commit_message>
adobe xd hifi vesion suunnittelua
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C51730-F070-4656-87A0-CFB29F4290BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAFB732-A98B-441A-949C-64CAC892AED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Päivä</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Adobe XD:llä sivujen hifi version suunnittelemistsa</t>
+  </si>
+  <si>
+    <t>Adobe XD:llä hifi version tekemistä ja logon uusiminen</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,10 +1152,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="3"/>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B42" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -1243,7 +1252,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="6">
         <f>SUM(B$2:B$59)</f>
-        <v>119.75</v>
+        <v>126.25</v>
       </c>
       <c r="C60" s="3"/>
     </row>

</xml_diff>

<commit_message>
html sivujen ja css:n toteuttamista
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA816D63-BB90-4DAB-AE3C-60F84A237384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5378C9A9-5CF1-446E-92DA-AA9882A1F693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Päivä</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Html pohjat valmiiks</t>
+  </si>
+  <si>
+    <t>Html sivujen ja css:n toteuttamista</t>
   </si>
 </sst>
 </file>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,9 +1195,15 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B45" s="6">
+        <v>7</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -1270,7 +1279,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="6">
         <f>SUM(B$2:B$59)</f>
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C60" s="3"/>
     </row>

</xml_diff>

<commit_message>
Landing page css: footer ja content
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5378C9A9-5CF1-446E-92DA-AA9882A1F693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F0E9A8-C296-4BD9-A391-8CB0354439E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27360" yWindow="720" windowWidth="21600" windowHeight="11385" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Päivä</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Html sivujen ja css:n toteuttamista</t>
+  </si>
+  <si>
+    <t>Landing page css: footer ja content</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,9 +1209,15 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="3"/>
+      <c r="A46" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B46" s="6">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -1279,7 +1288,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="6">
         <f>SUM(B$2:B$59)</f>
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C60" s="3"/>
     </row>

</xml_diff>

<commit_message>
html done ja css pääosin
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40D5DAA-5D4B-431E-84A2-85A2D19FAE3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FFF84C-F60F-4871-A0AF-9526DE82DF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18930" yWindow="2595" windowWidth="8625" windowHeight="9990" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Päivä</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>CSS: responsiivisuutta paikka sivu</t>
+  </si>
+  <si>
+    <t>CSS: responsiivisuus käyttäjä asetus sivuja</t>
+  </si>
+  <si>
+    <t>html done ja css pääosin</t>
   </si>
 </sst>
 </file>
@@ -715,7 +721,7 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,14 +1282,26 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="3"/>
+      <c r="A51" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B51" s="6">
+        <v>4</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="3"/>
+      <c r="A52" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B52" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -1329,7 +1347,7 @@
       <c r="A61" s="2"/>
       <c r="B61" s="6">
         <f>SUM(B$2:B$60)</f>
-        <v>163.5</v>
+        <v>170</v>
       </c>
       <c r="C61" s="3"/>
     </row>

</xml_diff>

<commit_message>
html:n ja scss:n viemistä reactiin + komponentteihin jakoa
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FFF84C-F60F-4871-A0AF-9526DE82DF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F47931-A53D-4262-94F5-20F0B93F4612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18930" yWindow="2595" windowWidth="8625" windowHeight="9990" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="-24435" yWindow="2190" windowWidth="14130" windowHeight="10395" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Päivä</t>
   </si>
@@ -176,28 +176,34 @@
     <t>Html pohjat valmiiks</t>
   </si>
   <si>
-    <t>Html sivujen ja css:n toteuttamista</t>
-  </si>
-  <si>
-    <t>Landing page css: footer ja content</t>
-  </si>
-  <si>
-    <t>CSS: responsiivisuutta</t>
-  </si>
-  <si>
-    <t>CSS: sivuja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSS: Responsiivisuus käyttäjä ja paikka sivu done </t>
-  </si>
-  <si>
-    <t>CSS: responsiivisuutta paikka sivu</t>
-  </si>
-  <si>
-    <t>CSS: responsiivisuus käyttäjä asetus sivuja</t>
-  </si>
-  <si>
     <t>html done ja css pääosin</t>
+  </si>
+  <si>
+    <t>SCSS: responsiivisuus käyttäjä asetus sivuja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCSS: Responsiivisuus käyttäjä ja paikka sivu done </t>
+  </si>
+  <si>
+    <t>SCSS: responsiivisuutta paikka sivu</t>
+  </si>
+  <si>
+    <t>SCSS: sivuja</t>
+  </si>
+  <si>
+    <t>SCSS: responsiivisuutta</t>
+  </si>
+  <si>
+    <t>Landing page scss: footer ja content</t>
+  </si>
+  <si>
+    <t>Html sivujen ja scss:n toteuttamista</t>
+  </si>
+  <si>
+    <t>html:n ja scss:n siirto Reactiin</t>
+  </si>
+  <si>
+    <t>html:n ja scss:n siirto Reactiin + jakamista komponentteihin</t>
   </si>
 </sst>
 </file>
@@ -720,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1229,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,7 +1251,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,7 +1262,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1267,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,7 +1284,7 @@
         <v>2.5</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1289,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,18 +1306,30 @@
         <v>2.5</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="3"/>
+      <c r="A53" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B53" s="6">
+        <v>3</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B54" s="6">
+        <v>1</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1347,7 +1365,7 @@
       <c r="A61" s="2"/>
       <c r="B61" s="6">
         <f>SUM(B$2:B$60)</f>
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C61" s="3"/>
     </row>

</xml_diff>

<commit_message>
Frontin jakamista ja backendin malleihin lisäystä
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA9F8B5-6848-417C-8696-22663F3FCFA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284140B4-6331-4EF5-AA73-0683EC569540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24435" yWindow="2175" windowWidth="14070" windowHeight="10410" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="-14730" yWindow="1320" windowWidth="14070" windowHeight="10410" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Päivä</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Frontin työstöä</t>
+  </si>
+  <si>
+    <t>Frontin jakamista ja backendin malleihin lisäystä</t>
   </si>
 </sst>
 </file>
@@ -736,7 +739,7 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,9 +1377,15 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B58" s="6">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -1397,7 +1406,7 @@
       <c r="A62" s="2"/>
       <c r="B62" s="6">
         <f>SUM(B$2:B$61)</f>
-        <v>183.5</v>
+        <v>184.5</v>
       </c>
       <c r="C62" s="3"/>
     </row>

</xml_diff>

<commit_message>
Viimeiset 20h + deploy
</commit_message>
<xml_diff>
--- a/Työaikakirjanpito_fullstackHt.xlsx
+++ b/Työaikakirjanpito_fullstackHt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kurssit\FullStackHarjoitustyo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kouluhommat\ClimbingFinland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284140B4-6331-4EF5-AA73-0683EC569540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D974D08C-7F12-46D6-A4D8-2FF6979A377A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14730" yWindow="1320" windowWidth="14070" windowHeight="10410" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{50B33E53-4B49-48DC-982C-197E5C8FA7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Päivä</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>Frontin jakamista ja backendin malleihin lisäystä</t>
+  </si>
+  <si>
+    <t>14.2.2021 -14.3.2021</t>
+  </si>
+  <si>
+    <t>Pitkän ajan jälkeen projektin puhhistamista ja deployaaminen</t>
   </si>
 </sst>
 </file>
@@ -738,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222E630B-CF39-4DAE-A968-DC7A76C0B9F6}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,10 +1393,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="3"/>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="6">
+        <v>20</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1406,7 +1418,7 @@
       <c r="A62" s="2"/>
       <c r="B62" s="6">
         <f>SUM(B$2:B$61)</f>
-        <v>184.5</v>
+        <v>204.5</v>
       </c>
       <c r="C62" s="3"/>
     </row>

</xml_diff>